<commit_message>
Clean node evaluation processing.
</commit_message>
<xml_diff>
--- a/data/mappers/node_evaluation_vissim_report_mapping.xlsx
+++ b/data/mappers/node_evaluation_vissim_report_mapping.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abibeka\Github\Tobin Bridge Vissim Processing\data\mappers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA52CAE-E642-4ECC-8F65-DEB828701047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FF24B9-A8A9-4C18-B932-28F1F345FF09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4EEC3B63-2907-4D6D-8AF0-8B40ADC5D7B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21864" windowHeight="13176" activeTab="2" xr2:uid="{4EEC3B63-2907-4D6D-8AF0-8B40ADC5D7B7}"/>
   </bookViews>
   <sheets>
     <sheet name="vissim_report_convertion" sheetId="1" r:id="rId1"/>
     <sheet name="deduplicate_movements" sheetId="2" r:id="rId2"/>
+    <sheet name="node_types" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="127">
   <si>
     <t>direction_results</t>
   </si>
@@ -407,6 +408,15 @@
   </si>
   <si>
     <t>NWB MA 3</t>
+  </si>
+  <si>
+    <t>intersection_type</t>
+  </si>
+  <si>
+    <t>Signalized</t>
+  </si>
+  <si>
+    <t>twsc</t>
   </si>
 </sst>
 </file>
@@ -422,18 +432,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -485,30 +489,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -526,6 +542,63 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -556,7 +629,52 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -585,37 +703,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -626,8 +719,6 @@
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -656,14 +747,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9CED0673-5A03-4330-B343-84BE1B2EF9BC}" name="Table1" displayName="Table1" ref="A1:E12" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9CED0673-5A03-4330-B343-84BE1B2EF9BC}" name="Table1" displayName="Table1" ref="A1:E12" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:E12" xr:uid="{D0009935-82AE-4D9E-A12D-E81A08FD2009}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B2EA7CCF-D201-4464-A4A6-5753DA0ED25F}" name="node_no" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{21D3F657-5776-4BED-9A8B-FBCE2C52F8BB}" name="movement_direction" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{4C9CECDD-0AF2-4F0B-A2F9-5E53CA791932}" name="movement_direction_unique"/>
-    <tableColumn id="4" xr3:uid="{A955384D-2EA8-4552-BD50-DCC68799798E}" name="from_link" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{F408AD12-55E3-4355-A010-0B3BD255BAA7}" name="to_link" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B2EA7CCF-D201-4464-A4A6-5753DA0ED25F}" name="node_no" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{21D3F657-5776-4BED-9A8B-FBCE2C52F8BB}" name="movement_direction" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{4C9CECDD-0AF2-4F0B-A2F9-5E53CA791932}" name="movement_direction_unique" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{A955384D-2EA8-4552-BD50-DCC68799798E}" name="from_link" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{F408AD12-55E3-4355-A010-0B3BD255BAA7}" name="to_link" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7A172F30-4ABE-481F-96E3-1E3964D9BFFF}" name="Table3" displayName="Table3" ref="A1:B19" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B19" xr:uid="{01382732-1F04-417D-BCCF-1BB2E848AF38}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{B8A5CC37-DC65-443D-91D8-B7DBA6588226}" name="node_no" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{4B32E5B1-CA05-4B71-B5A7-74FF48B5E36C}" name="intersection_type" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -968,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA83A6C2-E793-48C7-9267-43E16B54640C}">
   <dimension ref="A1:C119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2301,8 +2403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368A3629-2649-458F-B1E2-576370896C83}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2313,207 +2415,380 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="5" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FDF1FD-5AD3-461B-8988-CF3807561F99}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>